<commit_message>
Data driven - 2 ( not able to run test data driven)
</commit_message>
<xml_diff>
--- a/mmt/Excel/login.xlsx
+++ b/mmt/Excel/login.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>test1@gmail.com</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>dixit123</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +385,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,7 +415,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId2" display="dixit1234@"/>
     <hyperlink ref="A2" r:id="rId3"/>
     <hyperlink ref="B2" r:id="rId4"/>
     <hyperlink ref="A3" r:id="rId5"/>

</xml_diff>